<commit_message>
Added EmissionActivity to Connections, and MaxActivity to Fuels
Created project - test_emerging_tech, to act as a plact to store test cases for emerging technologies to make sure they are working before being introduced into larger models

Updated version #
</commit_message>
<xml_diff>
--- a/examples/baselines/data/data.xlsx
+++ b/examples/baselines/data/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC34D81E-1D36-4427-AD12-A04349A19B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43008D3B-12D9-4059-90B9-34CBC50B932E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="249">
   <si>
     <t>connection</t>
   </si>
@@ -1469,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,7 +1489,7 @@
     <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1535,8 +1535,14 @@
       <c r="O1" s="29" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1582,8 +1588,14 @@
       <c r="O2" s="30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -1607,7 +1619,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -1633,7 +1645,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1659,7 +1671,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1693,7 +1705,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -1719,7 +1731,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1760,7 +1772,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -1774,7 +1786,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -2635,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2660,34 +2672,34 @@
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="4" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2698,34 +2710,34 @@
       <c r="B2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="3" t="s">
         <v>76</v>
       </c>
     </row>
@@ -7071,10 +7083,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:P2"/>
+      <selection activeCell="L1" sqref="L1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7087,11 +7099,12 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" customWidth="1"/>
+    <col min="12" max="13" width="13.44140625" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7125,23 +7138,29 @@
       <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="P1" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="Q1" s="29" t="s">
         <v>247</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="R1" s="29" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -7175,23 +7194,29 @@
       <c r="K2" t="s">
         <v>71</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" t="s">
         <v>66</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="P2" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="O2" s="30" t="s">
+      <c r="Q2" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="P2" s="30" t="s">
+      <c r="R2" s="30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -7223,17 +7248,17 @@
       <c r="K3" t="s">
         <v>198</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>183</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>196</v>
       </c>
@@ -7261,17 +7286,17 @@
       <c r="K4" t="s">
         <v>198</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>30</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>183</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>2021</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -7303,14 +7328,14 @@
       <c r="K5" t="s">
         <v>198</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>30</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -7342,14 +7367,14 @@
       <c r="K6" t="s">
         <v>198</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>30</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -7362,14 +7387,14 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>30</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>200</v>
       </c>
@@ -7397,14 +7422,14 @@
       <c r="K8" t="s">
         <v>198</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>30</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>199</v>
       </c>
@@ -7432,14 +7457,14 @@
       <c r="K9" t="s">
         <v>198</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>30</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>204</v>
       </c>
@@ -7461,14 +7486,14 @@
       <c r="H10" t="s">
         <v>245</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>30</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>205</v>
       </c>
@@ -7490,14 +7515,14 @@
       <c r="H11" t="s">
         <v>245</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>30</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>212</v>
       </c>
@@ -7519,14 +7544,14 @@
       <c r="H12" t="s">
         <v>245</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>30</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>206</v>
       </c>
@@ -7548,14 +7573,14 @@
       <c r="H13" t="s">
         <v>245</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>30</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O13" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>207</v>
       </c>
@@ -7577,10 +7602,10 @@
       <c r="H14" t="s">
         <v>245</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>30</v>
       </c>
-      <c r="M14" t="s">
+      <c r="O14" t="s">
         <v>183</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added MaxCapacity and Ref_MaxCapacity inputs for Fuels
Made corresponding updates throughout examples and in va_emerging_tech project
</commit_message>
<xml_diff>
--- a/examples/baselines/data/data.xlsx
+++ b/examples/baselines/data/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32520121-8255-4768-BD1D-B5AFE4713ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0702A145-D3C1-4102-B0C0-9F643F55FCD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="253">
   <si>
     <t>connection</t>
   </si>
@@ -1523,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1546,7 +1546,7 @@
     <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1598,8 +1598,14 @@
       <c r="Q1" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1651,8 +1657,14 @@
       <c r="Q2" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -1685,7 +1697,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -1720,7 +1732,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1755,7 +1767,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1781,7 +1793,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1811,7 +1823,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -1846,7 +1858,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1891,7 +1903,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -1917,7 +1929,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -5112,7 +5124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB94AB1C-AA63-4D03-BFF0-AB1AB7BB172A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>